<commit_message>
changed the swipable lists to a context menu
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moonslic3r.DESKTOP-N81PI1L\listicle\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29CD5B1-9E0D-4740-9797-4753D124F990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A65EF2A-485E-4B38-8645-FF0416B69BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>Item</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Spekko Rice</t>
   </si>
   <si>
-    <t>170,00</t>
-  </si>
-  <si>
     <t>Candy Tops Eclairs 100g Choc</t>
   </si>
   <si>
@@ -179,13 +176,43 @@
   </si>
   <si>
     <t>180,00</t>
+  </si>
+  <si>
+    <t>Sasko Cake Flour</t>
+  </si>
+  <si>
+    <t>Lobels Original Mints 100s</t>
+  </si>
+  <si>
+    <t>Amajoya candy 50s</t>
+  </si>
+  <si>
+    <t>Beacon fizzers 100s</t>
+  </si>
+  <si>
+    <t>Sour Fruit Bars (Soapies) 20s</t>
+  </si>
+  <si>
+    <t>Broadway Heartbeat Candy 166s</t>
+  </si>
+  <si>
+    <t>Champion Toffees 112s</t>
+  </si>
+  <si>
+    <t>Milkit Lolipops Asstorted 48s</t>
+  </si>
+  <si>
+    <t>Truda Spookies 12x50g</t>
+  </si>
+  <si>
+    <t>Truda Go-Slos 12x100g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -196,6 +223,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,9 +253,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,23 +477,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="20" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -464,7 +501,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -472,7 +509,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -480,7 +517,7 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -488,7 +525,7 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -496,7 +533,7 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -504,7 +541,7 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -512,7 +549,7 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -520,168 +557,248 @@
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+      <c r="B9" s="2">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="B30" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the css for larger devices
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moonslic3r.DESKTOP-N81PI1L\listicle\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A65EF2A-485E-4B38-8645-FF0416B69BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D398A628-7A30-4CE1-964D-C8AE5738928A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t>Item</t>
   </si>
@@ -206,13 +206,34 @@
   </si>
   <si>
     <t>Truda Go-Slos 12x100g</t>
+  </si>
+  <si>
+    <t>115,00</t>
+  </si>
+  <si>
+    <t>25,00</t>
+  </si>
+  <si>
+    <t>57,00</t>
+  </si>
+  <si>
+    <t>28,00</t>
+  </si>
+  <si>
+    <t>39,00</t>
+  </si>
+  <si>
+    <t>32,00</t>
+  </si>
+  <si>
+    <t>160,00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -228,6 +249,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,12 +281,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,8 +510,8 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -489,7 +520,7 @@
     <col min="2" max="2" width="20" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -505,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -513,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -521,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -529,7 +560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -537,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -545,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -553,15 +584,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -569,7 +600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -577,7 +608,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -585,7 +616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -593,7 +624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -601,7 +632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -609,7 +640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -617,7 +648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -625,7 +656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -633,7 +664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -641,7 +672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -649,7 +680,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -657,7 +688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -665,7 +696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
@@ -673,7 +704,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -681,7 +712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -689,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -697,7 +728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -705,7 +736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -713,7 +744,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -725,80 +756,80 @@
       <c r="A30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="3">
-        <v>115</v>
+      <c r="B30" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="3">
-        <v>25</v>
+      <c r="B31" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="3">
-        <v>15</v>
+      <c r="B32" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="3">
-        <v>57</v>
+      <c r="B33" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="3">
-        <v>28</v>
+      <c r="B34" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="3">
-        <v>54</v>
+      <c r="B35" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="3">
-        <v>50</v>
+      <c r="B36" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="3">
-        <v>39</v>
+      <c r="B37" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="3">
-        <v>32</v>
+      <c r="B38" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="3">
-        <v>50</v>
+      <c r="B39" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>